<commit_message>
Revert "needssupersense and ssupdate.md updates"
This reverts commit 5e63ca2356d0a3e1d6045e686b55b0bc6fd537f8.
</commit_message>
<xml_diff>
--- a/needssupersense.xlsx
+++ b/needssupersense.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanmannion/streuslefork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C945C2-9B93-7E4E-BB43-4CB669E0677E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4F2081-70A5-9845-97F7-6B4AFD363561}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{B7556B33-DA83-C149-A2E9-9360D634E56C}"/>
+    <workbookView xWindow="-38400" yWindow="-8600" windowWidth="38400" windowHeight="21140" xr2:uid="{B7556B33-DA83-C149-A2E9-9360D634E56C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ssaudit" localSheetId="0">Sheet1!$A$1:$T$104</definedName>
+    <definedName name="ssaudit" localSheetId="0">Sheet1!$A$1:$T$131</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="483">
   <si>
     <t># _sentid</t>
   </si>
@@ -84,9 +84,30 @@
     <t>_context</t>
   </si>
   <si>
+    <t>reviews-003418-0009</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>say</t>
+  </si>
+  <si>
+    <t>I eventually decided to just pay the balance even though the doctor has already been paid , but now the collection agency is trying to &gt;&gt; say &lt;&lt; another reversal of $ 160.00 has come through .</t>
+  </si>
+  <si>
+    <t>reviews-007403-0004</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
+    <t>personalize</t>
+  </si>
+  <si>
+    <t>I offer compassionate , approachable and &gt;&gt; personalized &lt;&lt; counseling services .</t>
+  </si>
+  <si>
     <t>reviews-007403-0007</t>
   </si>
   <si>
@@ -99,6 +120,18 @@
     <t>I am a &gt;&gt; preferred &lt;&lt; provider with most insurance companies .</t>
   </si>
   <si>
+    <t>reviews-008585-0007</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Thanks &lt;&lt; Bud for all of your help and taking time away from your family that evening .</t>
+  </si>
+  <si>
     <t>reviews-009775-0003</t>
   </si>
   <si>
@@ -135,6 +168,18 @@
     <t>I 'm pretty sure for the cast that it was &gt;&gt; the other way around &lt;&lt; .</t>
   </si>
   <si>
+    <t>reviews-018548-0011</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>crush</t>
+  </si>
+  <si>
+    <t>it runs you about 4 bucks and it deals &gt;&gt; crushing &lt;&lt; blows to hunger .</t>
+  </si>
+  <si>
     <t>reviews-018562-0004</t>
   </si>
   <si>
@@ -159,6 +204,18 @@
     <t>Their selection is random , so what they have on a &gt;&gt; given &lt;&lt; week might never be available again at the store .</t>
   </si>
   <si>
+    <t>reviews-020992-0003</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>At 3:15 am on night &gt;&gt; # &lt;&lt; 2 , the fire alarm and strobe light activated in my room .</t>
+  </si>
+  <si>
     <t>reviews-030875-0003</t>
   </si>
   <si>
@@ -183,9 +240,27 @@
     <t>printing , printing , copies , printing , copies , &gt;&gt; printing &lt;&lt; ,</t>
   </si>
   <si>
+    <t>reviews-034813-0003</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
+    <t>signature</t>
+  </si>
+  <si>
+    <t>This place is awesome , with a great ambiance and cool décor , and the food is scrumptious ( and especially their &gt;&gt; signature &lt;&lt; banana split ) .</t>
+  </si>
+  <si>
+    <t>reviews-036133-0001</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Bit &lt;&lt; sketchy , sporadic delivery times</t>
+  </si>
+  <si>
     <t>reviews-036133-0019</t>
   </si>
   <si>
@@ -255,6 +330,18 @@
     <t>We tried 4 different style of donuts , they were all the same &gt;&gt; when it came to &lt;&lt; quality .</t>
   </si>
   <si>
+    <t>reviews-048363-0012</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>I trust you and believe that you 'll be able to handle this and all you have to &gt;&gt; do &lt;&lt; is to reciprocate !</t>
+  </si>
+  <si>
     <t>reviews-048363-0015</t>
   </si>
   <si>
@@ -357,6 +444,15 @@
     <t>reviews-077414-0004</t>
   </si>
   <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+  <si>
+    <t>While I hope I do n't have any &gt;&gt; need &lt;&lt; for a lawyer anytime soon , if I do I 'll definitely use this firm again .</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
@@ -549,6 +645,15 @@
     <t>We also liked the &gt;&gt; way &lt;&lt; that Ray checked on the job every day .</t>
   </si>
   <si>
+    <t>reviews-125522-0003</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>Calls are now forwarded to Malcolm Smith Motorsports down the &gt;&gt; road &lt;&lt; .</t>
+  </si>
+  <si>
     <t>reviews-127157-0004</t>
   </si>
   <si>
@@ -561,9 +666,18 @@
     <t>One guy is a little surley , but &gt;&gt; who gives a crap &lt;&lt; as long as your car 's work is outstanding .</t>
   </si>
   <si>
+    <t>reviews-134741-0003</t>
+  </si>
+  <si>
     <t>16</t>
   </si>
   <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>It made me feel good to see people work so hard to take care of &gt;&gt; others &lt;&lt; belongings .</t>
+  </si>
+  <si>
     <t>reviews-139152-0003</t>
   </si>
   <si>
@@ -579,6 +693,15 @@
     <t>But she did a fabulous job letting me know what she was doing at all times and styled my hair in a &gt;&gt; way &lt;&lt; i could do it at home .</t>
   </si>
   <si>
+    <t>reviews-158335-0006</t>
+  </si>
+  <si>
+    <t>grey</t>
+  </si>
+  <si>
+    <t>&gt;&gt; grey &lt;&lt; shirt " mark " of course with this type behavior he could have been wearing someon else s clothing .....</t>
+  </si>
+  <si>
     <t>reviews-163703-0002</t>
   </si>
   <si>
@@ -591,6 +714,18 @@
     <t>Cheap Hotel Rome - thanks for finding us a hotel at the &gt;&gt; last minute &lt;&lt; .</t>
   </si>
   <si>
+    <t>reviews-165032-0002</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>We went through six photographers to find the right photographers that would represent our firm in the &gt;&gt; light &lt;&lt; we wished to and Michael and his team made that happen .</t>
+  </si>
+  <si>
     <t>reviews-166983-0001</t>
   </si>
   <si>
@@ -711,6 +846,15 @@
     <t>Service was &gt;&gt; a touch &lt;&lt; slow , but friendly .</t>
   </si>
   <si>
+    <t>reviews-219262-0008</t>
+  </si>
+  <si>
+    <t>thank</t>
+  </si>
+  <si>
+    <t>My family and I &gt;&gt; thank &lt;&lt; you !!!!!!!!!!</t>
+  </si>
+  <si>
     <t>reviews-224117-0001</t>
   </si>
   <si>
@@ -729,6 +873,15 @@
     <t>All to the &gt;&gt; good &lt;&lt; .</t>
   </si>
   <si>
+    <t>reviews-228944-0004</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>They are the only place I would take my car &gt;&gt; peiod &lt;&lt; .</t>
+  </si>
+  <si>
     <t>reviews-229410-0009</t>
   </si>
   <si>
@@ -789,6 +942,12 @@
     <t>&gt;&gt; STAY AWAY &lt;&lt;</t>
   </si>
   <si>
+    <t>reviews-241855-0002</t>
+  </si>
+  <si>
+    <t>I sometimes go into this store just for something to &gt;&gt; do &lt;&lt; on a sunday afternoon .</t>
+  </si>
+  <si>
     <t>reviews-243799-0002</t>
   </si>
   <si>
@@ -816,6 +975,12 @@
     <t>With all the child predators out there , a busy road , cars speeding by ...... and you are going to let some 4 / 5 year olds wonder around cause you 're &gt;&gt; money hungry &lt;&lt; ?</t>
   </si>
   <si>
+    <t>reviews-260640-0007</t>
+  </si>
+  <si>
+    <t>Whether they pay me or not , if their parents get into an accident , stuck in traffic , etc. THE LAST THING I WOULD &gt;&gt; DO &lt;&lt; IS LET A CHILD GET RAPED BECAUSE I WAS N'T PAID .</t>
+  </si>
+  <si>
     <t>reviews-263630-0008</t>
   </si>
   <si>
@@ -834,6 +999,15 @@
     <t>VCU has the &gt;&gt; # 1 &lt;&lt; art school in America , and EXCELS in healthcare and medical schooling .</t>
   </si>
   <si>
+    <t>reviews-268673-0003</t>
+  </si>
+  <si>
+    <t>shelf</t>
+  </si>
+  <si>
+    <t>To my surprise $ 20 deposit .... New movies not on &gt;&gt; shelf &lt;&lt; .. under the counter for Telugu Speaking people only ... or people who spend $ 30 or more groceries ..</t>
+  </si>
+  <si>
     <t>reviews-278775-0005</t>
   </si>
   <si>
@@ -846,6 +1020,15 @@
     <t>We were familiar with Search Engine Optimization strategies , but new nothing about Social Media - we just heard that it was &gt;&gt; the next big thing &lt;&lt; .</t>
   </si>
   <si>
+    <t>reviews-279070-0002</t>
+  </si>
+  <si>
+    <t>business</t>
+  </si>
+  <si>
+    <t>Happened on to this place while out of town on &gt;&gt; business &lt;&lt; , and it was great !</t>
+  </si>
+  <si>
     <t>reviews-281976-0004</t>
   </si>
   <si>
@@ -864,6 +1047,21 @@
     <t>&gt;&gt; Way to go &lt;&lt; !</t>
   </si>
   <si>
+    <t>reviews-306740-0001</t>
+  </si>
+  <si>
+    <t>tutoring</t>
+  </si>
+  <si>
+    <t>Miami 's best &gt;&gt; tutoring &lt;&lt; service !</t>
+  </si>
+  <si>
+    <t>reviews-307250-0002</t>
+  </si>
+  <si>
+    <t>Worst buffet &gt;&gt; period &lt;&lt; by far .</t>
+  </si>
+  <si>
     <t>reviews-307250-0003</t>
   </si>
   <si>
@@ -933,6 +1131,12 @@
     <t>I look at some of these other comments &amp; laugh because people think that &gt;&gt; the world revolves around &lt;&lt; them !</t>
   </si>
   <si>
+    <t>reviews-331662-0003</t>
+  </si>
+  <si>
+    <t>Everyone can get the &gt;&gt; signature &lt;&lt; dish with ingredients and spices that they want and have the fun of watching it cook .</t>
+  </si>
+  <si>
     <t>reviews-333243-0006</t>
   </si>
   <si>
@@ -954,9 +1158,24 @@
     <t>reviews-339176-0007</t>
   </si>
   <si>
+    <t>top notch</t>
+  </si>
+  <si>
+    <t>&gt;&gt; Top notch &lt;&lt; , all the way !</t>
+  </si>
+  <si>
     <t>Top notch , &gt;&gt; all the way &lt;&lt; !</t>
   </si>
   <si>
+    <t>reviews-342811-0001</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>Friendly &gt;&gt; staff &lt;&lt; , but definitely some problems</t>
+  </si>
+  <si>
     <t>reviews-346960-0002</t>
   </si>
   <si>
@@ -993,6 +1212,15 @@
     <t>&gt;&gt; Hands down &lt;&lt; , best place in the area !</t>
   </si>
   <si>
+    <t>reviews-357217-0001</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>A Definite &gt;&gt; No &lt;&lt;</t>
+  </si>
+  <si>
     <t>reviews-358063-0003</t>
   </si>
   <si>
@@ -1032,6 +1260,15 @@
     <t>Bramen Honda was &gt;&gt; a bit of a &lt;&lt; hassle .</t>
   </si>
   <si>
+    <t>reviews-369210-0006</t>
+  </si>
+  <si>
+    <t>world</t>
+  </si>
+  <si>
+    <t>Brickell Honda has been the best buying experience in the &gt;&gt; world &lt;&lt; .</t>
+  </si>
+  <si>
     <t>reviews-371300-0007</t>
   </si>
   <si>
@@ -1074,6 +1311,15 @@
     <t>so go and &gt;&gt; get &lt;&lt; dancing !!!!!!!!!!!!!!!!!!!!!!!!!</t>
   </si>
   <si>
+    <t>reviews-391012-0006</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>The craziest &gt;&gt; part &lt;&lt; is that they are n't even based locally at the city I 'm in - they just have ' teams ' in areas through the country .</t>
+  </si>
+  <si>
     <t>reviews-392826-0002</t>
   </si>
   <si>
@@ -1146,6 +1392,9 @@
     <t>V</t>
   </si>
   <si>
+    <t>n.LOCATION</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -1173,9 +1422,15 @@
     <t>going to' as AUX</t>
   </si>
   <si>
+    <t>SYM</t>
+  </si>
+  <si>
     <t>n.COMMUNICATION</t>
   </si>
   <si>
+    <t>attested</t>
+  </si>
+  <si>
     <t>n.FEELING</t>
   </si>
   <si>
@@ -1185,9 +1440,21 @@
     <t>N/DET</t>
   </si>
   <si>
+    <t>same as 'a bit'? Elision?</t>
+  </si>
+  <si>
+    <t>n.GROUP</t>
+  </si>
+  <si>
     <t>ADV</t>
   </si>
   <si>
+    <t>body, animal, person</t>
+  </si>
+  <si>
+    <t>n.PERSON</t>
+  </si>
+  <si>
     <t>v.communication</t>
   </si>
   <si>
@@ -1200,6 +1467,12 @@
     <t>v.cognition</t>
   </si>
   <si>
+    <t>how do I deal with these</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
     <t>N? ADJ?</t>
   </si>
   <si>
@@ -1215,70 +1488,31 @@
     <t>preppy, feels like n.LOCATION</t>
   </si>
   <si>
+    <t>n.MOTIVE</t>
+  </si>
+  <si>
     <t>unsure</t>
   </si>
   <si>
+    <t>PRON</t>
+  </si>
+  <si>
     <t>"all good"</t>
   </si>
   <si>
+    <t>down the road MWE?</t>
+  </si>
+  <si>
+    <t>n.ARTIFACT</t>
+  </si>
+  <si>
+    <t>DISC</t>
+  </si>
+  <si>
     <t>preppy but seems like quantity</t>
   </si>
   <si>
     <t>'</t>
-  </si>
-  <si>
-    <t>MWE</t>
-  </si>
-  <si>
-    <t>MWE - 'a couple'</t>
-  </si>
-  <si>
-    <t>DET</t>
-  </si>
-  <si>
-    <t>Whether they pay me or not , if their parents get into an accident , stuck in traffic , etc. THE LAST THING I WOULD &gt;&gt; DO &lt;&lt; IS LET A CHILD GET RAPED BECAUSE I WAS N'T PAID .</t>
-  </si>
-  <si>
-    <t>v.change</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>reviews-260640-0007</t>
-  </si>
-  <si>
-    <t>I sometimes go into this store just for something to &gt;&gt; do &lt;&lt; on a sunday afternoon .</t>
-  </si>
-  <si>
-    <t>reviews-241855-0002</t>
-  </si>
-  <si>
-    <t>I trust you and believe that you 'll be able to handle this and all you have to &gt;&gt; do &lt;&lt; is to reciprocate !</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>reviews-048363-0012</t>
-  </si>
-  <si>
-    <t>it runs you about 4 bucks and it deals &gt;&gt; crushing &lt;&lt; blows to hunger .</t>
-  </si>
-  <si>
-    <t>`j</t>
-  </si>
-  <si>
-    <t>crush</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>reviews-018548-0011</t>
   </si>
 </sst>
 </file>
@@ -1317,6 +1551,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1326,7 +1561,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1645,18 +1879,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A0DC6E-FE87-AD4B-A2DF-AD4DD981A944}">
-  <dimension ref="A1:G109"/>
+  <dimension ref="A1:G131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
@@ -1682,8 +1916,8 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>360</v>
+      <c r="C1" s="4" t="s">
+        <v>443</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1700,2027 +1934,2502 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>253</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="E2" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>255</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>362</v>
+        <v>223</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>454</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+        <v>309</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>150</v>
+        <v>394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>395</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>445</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>370</v>
-      </c>
+        <v>396</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>371</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="1" t="s">
-        <v>213</v>
+        <v>184</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>257</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>456</v>
+      </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>258</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>358</v>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1" t="s">
-        <v>26</v>
+        <v>259</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>250</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
-        <v>251</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G7" s="1" t="s">
-        <v>252</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>269</v>
+        <v>305</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>270</v>
+        <v>306</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>376</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>215</v>
+        <v>335</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>375</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
-        <v>216</v>
+        <v>336</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>465</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>164</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>464</v>
+      </c>
       <c r="D10" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>264</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>289</v>
+        <v>363</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>361</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>96</v>
+        <v>357</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>444</v>
+      </c>
       <c r="D12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>373</v>
-      </c>
+        <v>358</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>309</v>
+        <v>125</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>387</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>130</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>311</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>143</v>
+        <v>385</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>365</v>
+        <v>55</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>461</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>144</v>
+        <v>386</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>357</v>
+        <v>439</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>369</v>
+        <v>462</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>377</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>342</v>
+        <v>175</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>448</v>
+      </c>
       <c r="D16" s="1" t="s">
-        <v>343</v>
+        <v>176</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>359</v>
+        <v>439</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>374</v>
+        <v>453</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>224</v>
+        <v>318</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>319</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>459</v>
+      </c>
       <c r="G17" s="1" t="s">
-        <v>226</v>
+        <v>320</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>234</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C18" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>236</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>466</v>
+      </c>
       <c r="G18" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>119</v>
+        <v>424</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C19" s="4"/>
       <c r="D19" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+        <v>425</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="G19" s="1" t="s">
-        <v>122</v>
+        <v>426</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>221</v>
+        <v>275</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>388</v>
+        <v>104</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>445</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>389</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>260</v>
+        <v>285</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>365</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="C21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>261</v>
+        <v>287</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>364</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C22" s="3"/>
+        <v>152</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>445</v>
+      </c>
       <c r="D22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>366</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="G22" s="1" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>312</v>
+        <v>272</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="C23" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C23" s="4"/>
       <c r="D23" s="1" t="s">
-        <v>314</v>
+        <v>273</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>357</v>
+        <v>439</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>366</v>
+        <v>446</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>467</v>
+      </c>
       <c r="D24" s="1" t="s">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F24" s="1"/>
+        <v>468</v>
+      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>183</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>241</v>
+        <v>88</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
-        <v>182</v>
+        <v>90</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F25" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G25" s="1" t="s">
-        <v>242</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="1" t="s">
-        <v>182</v>
+        <v>90</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F26" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>194</v>
+        <v>303</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C27" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="1" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G27" s="1" t="s">
-        <v>196</v>
+        <v>304</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>321</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>378</v>
+        <v>201</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>448</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+        <v>322</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G28" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>368</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C29" s="4"/>
       <c r="D29" s="1" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="F29" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="G29" s="1" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>388</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>389</v>
+      </c>
+      <c r="C30" s="4"/>
       <c r="D30" s="1" t="s">
-        <v>53</v>
+        <v>390</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>359</v>
+        <v>439</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>374</v>
+        <v>449</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>54</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>226</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>218</v>
+        <v>294</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>384</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C32" s="4"/>
       <c r="D32" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E32" s="1"/>
+        <v>227</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1" t="s">
-        <v>220</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>123</v>
+        <v>413</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C33" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C33" s="4"/>
       <c r="D33" s="1" t="s">
-        <v>125</v>
+        <v>227</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>373</v>
+        <v>450</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1" t="s">
-        <v>126</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>127</v>
+        <v>239</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>183</v>
+      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="1" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>373</v>
+        <v>441</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>307</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>469</v>
+      </c>
       <c r="D35" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>373</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>332</v>
+        <v>231</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C36" s="3"/>
+        <v>232</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>451</v>
+      </c>
       <c r="D36" s="1" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>373</v>
+        <v>450</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>333</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>272</v>
+        <v>76</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C37" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>274</v>
+        <v>78</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>359</v>
+        <v>441</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>380</v>
+        <v>463</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>275</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>330</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>380</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>350</v>
+        <v>266</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>477</v>
+      </c>
       <c r="D39" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>367</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>352</v>
+        <v>268</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>322</v>
+        <v>209</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C40" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>324</v>
+        <v>210</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>364</v>
-      </c>
+        <v>470</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>325</v>
+        <v>211</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>297</v>
+        <v>155</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="C41" s="4"/>
       <c r="D41" s="1" t="s">
-        <v>298</v>
+        <v>157</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>367</v>
+        <v>460</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C42" s="4"/>
       <c r="D42" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E42" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>11</v>
+        <v>380</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C43" s="4"/>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>161</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>366</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>14</v>
+        <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>336</v>
+        <v>411</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C44" s="3"/>
+        <v>286</v>
+      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="1" t="s">
-        <v>337</v>
+        <v>161</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>366</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>382</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="C45" s="4"/>
       <c r="D45" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+        <v>340</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="G45" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>243</v>
+        <v>409</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>381</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C46" s="4"/>
       <c r="D46" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+        <v>340</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="G46" s="1" t="s">
-        <v>245</v>
+        <v>410</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>432</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C47" s="3"/>
+        <v>433</v>
+      </c>
+      <c r="C47" s="4"/>
       <c r="D47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="1"/>
+        <v>340</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>95</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>200</v>
+        <v>401</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C48" s="3"/>
+        <v>402</v>
+      </c>
+      <c r="C48" s="4"/>
       <c r="D48" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+        <v>403</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="G48" s="1" t="s">
-        <v>203</v>
+        <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>292</v>
+        <v>370</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="C49" s="4"/>
       <c r="D49" s="1" t="s">
-        <v>293</v>
+        <v>371</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>359</v>
+        <v>450</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>40</v>
+        <v>226</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>445</v>
+      </c>
       <c r="D50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>359</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C51" s="4"/>
       <c r="D51" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="G51" s="1" t="s">
-        <v>168</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>171</v>
+        <v>418</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C52" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="1" t="s">
-        <v>173</v>
+        <v>419</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>357</v>
+        <v>439</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>376</v>
+        <v>449</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C53" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>473</v>
+      </c>
       <c r="D53" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>377</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>296</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C54" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>472</v>
+      </c>
       <c r="D54" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>359</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1" t="s">
-        <v>138</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C55" s="3"/>
+        <v>122</v>
+      </c>
+      <c r="C55" s="4"/>
       <c r="D55" s="1" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>100</v>
+        <v>245</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C56" s="3"/>
+        <v>246</v>
+      </c>
+      <c r="C56" s="4"/>
       <c r="D56" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>379</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>266</v>
+        <v>360</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C57" s="4"/>
       <c r="D57" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E57" s="1"/>
+        <v>361</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>268</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>246</v>
+        <v>65</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C58" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="C58" s="4"/>
       <c r="D58" s="1" t="s">
-        <v>248</v>
+        <v>67</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>379</v>
+        <v>441</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1" t="s">
-        <v>249</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>383</v>
+        <v>156</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>445</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>370</v>
-      </c>
+        <v>205</v>
+      </c>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>278</v>
+        <v>212</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="C60" s="3"/>
+        <v>213</v>
+      </c>
+      <c r="C60" s="4"/>
       <c r="D60" s="1" t="s">
-        <v>280</v>
+        <v>214</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>357</v>
+        <v>439</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>358</v>
+        <v>465</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>326</v>
+        <v>216</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>362</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="C61" s="4"/>
       <c r="D61" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
+        <v>218</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G61" s="1" t="s">
-        <v>329</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="E62" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G62" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C63" s="3"/>
+        <v>168</v>
+      </c>
+      <c r="C63" s="4"/>
       <c r="D63" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>374</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C64" s="4"/>
       <c r="D64" s="1" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1" t="s">
-        <v>10</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>35</v>
+        <v>132</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C65" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="C65" s="4"/>
       <c r="D65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E65" s="1"/>
+        <v>134</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>470</v>
+      </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>154</v>
+        <v>332</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C66" s="3"/>
+        <v>223</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>445</v>
+      </c>
       <c r="D66" s="1" t="s">
-        <v>156</v>
+        <v>333</v>
       </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1" t="s">
-        <v>157</v>
+        <v>334</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>111</v>
+        <v>299</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="3"/>
+        <v>300</v>
+      </c>
+      <c r="C67" s="4"/>
       <c r="D67" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E67" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>470</v>
+      </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1" t="s">
-        <v>114</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>238</v>
+        <v>125</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="C68" s="4"/>
       <c r="D68" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
+        <v>127</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>474</v>
+      </c>
       <c r="G68" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>74</v>
+        <v>382</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="3"/>
+        <v>254</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>475</v>
+      </c>
       <c r="D69" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+        <v>383</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G69" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>197</v>
+        <v>281</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="3"/>
+        <v>282</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>475</v>
+      </c>
       <c r="D70" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="G70" s="1" t="s">
-        <v>199</v>
+        <v>284</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>80</v>
+        <v>344</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="3"/>
+        <v>345</v>
+      </c>
+      <c r="C71" s="4"/>
       <c r="D71" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+        <v>346</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G71" s="1" t="s">
-        <v>83</v>
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>88</v>
+        <v>405</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>385</v>
+        <v>406</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>445</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>90</v>
+        <v>407</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>303</v>
+        <v>147</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>386</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C73" s="4"/>
       <c r="D73" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+        <v>149</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="G73" s="1" t="s">
-        <v>306</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>339</v>
+        <v>200</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C74" s="3"/>
+        <v>201</v>
+      </c>
+      <c r="C74" s="4"/>
       <c r="D74" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>202</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="F74" s="1"/>
       <c r="G74" s="1" t="s">
-        <v>341</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C75" s="3"/>
+        <v>172</v>
+      </c>
+      <c r="C75" s="4"/>
       <c r="D75" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="G75" s="1" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>71</v>
+        <v>415</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C76" s="3"/>
+        <v>254</v>
+      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
+        <v>416</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="G76" s="1" t="s">
-        <v>73</v>
+        <v>417</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>78</v>
+        <v>269</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C77" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C77" s="4"/>
       <c r="D77" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E77" s="1"/>
+        <v>270</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>256</v>
+        <v>330</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="C78" s="3"/>
+        <v>254</v>
+      </c>
+      <c r="C78" s="4"/>
       <c r="D78" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>270</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>259</v>
+        <v>331</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="C79" s="4"/>
       <c r="D79" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C80" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C80" s="4"/>
       <c r="D80" s="1" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>285</v>
+        <v>54</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="C81" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C81" s="4"/>
       <c r="D81" s="1" t="s">
-        <v>287</v>
+        <v>56</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1" t="s">
-        <v>288</v>
+        <v>57</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C82" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="C82" s="4"/>
       <c r="D82" s="1" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C83" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>478</v>
+      </c>
       <c r="D83" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E83" s="1"/>
+        <v>194</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="F83" s="1"/>
       <c r="G83" s="1" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>282</v>
+        <v>143</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C84" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="C84" s="4"/>
       <c r="D84" s="1" t="s">
-        <v>283</v>
+        <v>145</v>
       </c>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1" t="s">
-        <v>284</v>
+        <v>146</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>227</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C85" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C85" s="4"/>
       <c r="D85" s="1" t="s">
-        <v>228</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>441</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="G85" s="1" t="s">
-        <v>229</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>208</v>
+        <v>311</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C86" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C86" s="4"/>
       <c r="D86" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+        <v>312</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>479</v>
+      </c>
       <c r="G86" s="1" t="s">
-        <v>211</v>
+        <v>313</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>353</v>
+        <v>58</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C87" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="C87" s="4"/>
       <c r="D87" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="G87" s="1" t="s">
-        <v>356</v>
+        <v>61</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>190</v>
+        <v>355</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C88" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C88" s="4"/>
       <c r="D88" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="G88" s="1" t="s">
-        <v>193</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>204</v>
+        <v>367</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C89" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="C89" s="4"/>
       <c r="D89" s="1" t="s">
-        <v>206</v>
+        <v>368</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>357</v>
+        <v>439</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>366</v>
+        <v>459</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>207</v>
+        <v>369</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>158</v>
+        <v>289</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C90" s="4"/>
       <c r="D90" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>357</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1" t="s">
-        <v>160</v>
+        <v>291</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C91" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="C91" s="4"/>
       <c r="D91" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>357</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>316</v>
+        <v>242</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C92" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="C92" s="4"/>
       <c r="D92" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>357</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1" t="s">
-        <v>317</v>
+        <v>244</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>263</v>
+        <v>109</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C93" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C93" s="4"/>
       <c r="D93" s="1" t="s">
-        <v>264</v>
+        <v>111</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1" t="s">
-        <v>265</v>
+        <v>112</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>104</v>
+        <v>260</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C94" s="3"/>
+        <v>110</v>
+      </c>
+      <c r="C94" s="4"/>
       <c r="D94" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
+        <v>261</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="G94" s="1" t="s">
-        <v>106</v>
+        <v>262</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>107</v>
+        <v>18</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C95" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="C95" s="4"/>
       <c r="D95" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E95" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>480</v>
+      </c>
       <c r="F95" s="1"/>
       <c r="G95" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C96" s="3"/>
+        <v>118</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>481</v>
+      </c>
       <c r="D96" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>276</v>
+        <v>376</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C97" s="3"/>
+        <v>377</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>482</v>
+      </c>
       <c r="D97" s="1" t="s">
-        <v>105</v>
+        <v>378</v>
       </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1" t="s">
-        <v>277</v>
+        <v>379</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>59</v>
+        <v>421</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C98" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C98" s="4"/>
       <c r="D98" s="1" t="s">
-        <v>61</v>
+        <v>422</v>
       </c>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1" t="s">
-        <v>62</v>
+        <v>423</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C99" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="C99" s="4"/>
       <c r="D99" s="1" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C100" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C100" s="4"/>
       <c r="D100" s="1" t="s">
-        <v>301</v>
+        <v>101</v>
       </c>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1" t="s">
-        <v>302</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>177</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C101" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C101" s="4"/>
       <c r="D101" s="1" t="s">
-        <v>179</v>
+        <v>101</v>
       </c>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>347</v>
+        <v>314</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="C102" s="3"/>
+        <v>315</v>
+      </c>
+      <c r="C102" s="4"/>
       <c r="D102" s="1" t="s">
-        <v>179</v>
+        <v>316</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="1" t="s">
-        <v>349</v>
+        <v>317</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C103" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="C103" s="4"/>
       <c r="D103" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>345</v>
+        <v>92</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C104" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="C104" s="4"/>
       <c r="D104" s="1" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="1" t="s">
-        <v>346</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C105" s="4"/>
+      <c r="D105" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E105" s="1"/>
+      <c r="F105" s="1"/>
+      <c r="G105" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>399</v>
+        <v>178</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C106" s="3"/>
+        <v>179</v>
+      </c>
+      <c r="C106" s="4"/>
       <c r="D106" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E106" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>391</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
       <c r="G106" s="1" t="s">
-        <v>397</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>396</v>
+        <v>220</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C107" s="3"/>
+        <v>23</v>
+      </c>
+      <c r="C107" s="4"/>
       <c r="D107" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="E107" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>391</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="E107" s="1"/>
+      <c r="F107" s="1"/>
       <c r="G107" s="1" t="s">
-        <v>395</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C108" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C108" s="4"/>
       <c r="D108" s="1" t="s">
-        <v>392</v>
+        <v>364</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>359</v>
+        <v>439</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>391</v>
+        <v>449</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>390</v>
+        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>404</v>
+        <v>348</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>402</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="C109" s="4"/>
       <c r="D109" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="E109" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="F109" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E109" s="1"/>
+      <c r="F109" s="1"/>
+      <c r="G109" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="4"/>
+      <c r="D110" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" s="4"/>
+      <c r="D111" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F111" s="1"/>
+      <c r="G111" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C112" s="4"/>
+      <c r="D112" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E112" s="1"/>
+      <c r="F112" s="1"/>
+      <c r="G112" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C113" s="4"/>
+      <c r="D113" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E113" s="1"/>
+      <c r="F113" s="1"/>
+      <c r="G113" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C114" s="4"/>
+      <c r="D114" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E114" s="1"/>
+      <c r="F114" s="1"/>
+      <c r="G114" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C116" s="4"/>
+      <c r="D116" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F116" s="1"/>
+      <c r="G116" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C117" s="4"/>
+      <c r="D117" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F117" s="1"/>
+      <c r="G117" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F118" s="1"/>
+      <c r="G118" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E119" s="1"/>
+      <c r="F119" s="1"/>
+      <c r="G119" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C120" s="4"/>
+      <c r="D120" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E120" s="1"/>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C121" s="4"/>
+      <c r="D121" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E121" s="1"/>
+      <c r="F121" s="1"/>
+      <c r="G121" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C122" s="4"/>
+      <c r="D122" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E122" s="1"/>
+      <c r="F122" s="1"/>
+      <c r="G122" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" s="4"/>
+      <c r="D123" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
+      <c r="G123" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C124" s="4"/>
+      <c r="D124" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E124" s="1"/>
+      <c r="F124" s="1"/>
+      <c r="G124" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C125" s="4"/>
+      <c r="D125" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E125" s="1"/>
+      <c r="F125" s="1"/>
+      <c r="G125" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C126" s="4"/>
+      <c r="D126" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="G127" s="1" t="s">
         <v>400</v>
       </c>
     </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C129" s="4"/>
+      <c r="D129" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C130" s="4"/>
+      <c r="D130" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C131" s="4"/>
+      <c r="D131" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G104">
-    <sortCondition ref="D2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G131">
+    <sortCondition ref="D3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>